<commit_message>
Create report for the measured matrix
</commit_message>
<xml_diff>
--- a/src/relatorio/demo.xlsx
+++ b/src/relatorio/demo.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="13">
+  <si>
+    <t>Measured</t>
+  </si>
   <si>
     <t>swimming</t>
   </si>
@@ -38,6 +41,9 @@
   </si>
   <si>
     <t>prevalencia</t>
+  </si>
+  <si>
+    <t>Maximum</t>
   </si>
   <si>
     <t>not swimming</t>
@@ -378,35 +384,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C9:M39"/>
+  <dimension ref="C8:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="8" spans="3:13">
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="9" spans="3:13">
       <c r="D9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="3:13">
       <c r="C10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -418,7 +432,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>4</v>
@@ -432,7 +446,7 @@
     </row>
     <row r="11" spans="3:13">
       <c r="C11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -444,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -458,7 +472,7 @@
     </row>
     <row r="12" spans="3:13">
       <c r="C12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -470,7 +484,7 @@
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -484,34 +498,34 @@
     </row>
     <row r="14" spans="3:13">
       <c r="C14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" t="s">
         <v>5</v>
       </c>
-      <c r="F14" t="s">
+      <c r="K14" t="s">
         <v>6</v>
       </c>
-      <c r="G14" t="s">
+      <c r="L14" t="s">
         <v>7</v>
       </c>
-      <c r="I14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" t="s">
-        <v>5</v>
-      </c>
-      <c r="L14" t="s">
-        <v>6</v>
-      </c>
       <c r="M14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="3:13">
@@ -546,23 +560,31 @@
         <v>1</v>
       </c>
     </row>
+    <row r="17" spans="3:13">
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="18" spans="3:13">
       <c r="D18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="3:13">
       <c r="C19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -571,7 +593,7 @@
         <v>4</v>
       </c>
       <c r="I19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
         <v>4</v>
@@ -582,7 +604,7 @@
     </row>
     <row r="20" spans="3:13">
       <c r="C20" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -591,7 +613,7 @@
         <v>3</v>
       </c>
       <c r="I20" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -602,34 +624,34 @@
     </row>
     <row r="22" spans="3:13">
       <c r="C22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" t="s">
         <v>5</v>
       </c>
-      <c r="F22" t="s">
+      <c r="K22" t="s">
         <v>6</v>
       </c>
-      <c r="G22" t="s">
+      <c r="L22" t="s">
         <v>7</v>
       </c>
-      <c r="I22" t="s">
-        <v>3</v>
-      </c>
-      <c r="J22" t="s">
-        <v>4</v>
-      </c>
-      <c r="K22" t="s">
-        <v>5</v>
-      </c>
-      <c r="L22" t="s">
-        <v>6</v>
-      </c>
       <c r="M22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="3:13">
@@ -664,23 +686,31 @@
         <v>0.09090910000000001</v>
       </c>
     </row>
+    <row r="25" spans="3:13">
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="26" spans="3:13">
       <c r="D26" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J26" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K26" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="3:13">
       <c r="C27" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -689,7 +719,7 @@
         <v>4</v>
       </c>
       <c r="I27" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J27">
         <v>4</v>
@@ -700,7 +730,7 @@
     </row>
     <row r="28" spans="3:13">
       <c r="C28" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D28">
         <v>4</v>
@@ -709,7 +739,7 @@
         <v>5</v>
       </c>
       <c r="I28" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -720,34 +750,34 @@
     </row>
     <row r="30" spans="3:13">
       <c r="C30" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" t="s">
         <v>5</v>
       </c>
-      <c r="F30" t="s">
+      <c r="K30" t="s">
         <v>6</v>
       </c>
-      <c r="G30" t="s">
+      <c r="L30" t="s">
         <v>7</v>
       </c>
-      <c r="I30" t="s">
-        <v>3</v>
-      </c>
-      <c r="J30" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30" t="s">
-        <v>5</v>
-      </c>
-      <c r="L30" t="s">
-        <v>6</v>
-      </c>
       <c r="M30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="3:13">
@@ -782,23 +812,31 @@
         <v>0.384615</v>
       </c>
     </row>
+    <row r="33" spans="3:13">
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="34" spans="3:13">
       <c r="D34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="3:13">
       <c r="C35" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -807,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J35">
         <v>3</v>
@@ -818,7 +856,7 @@
     </row>
     <row r="36" spans="3:13">
       <c r="C36" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -827,7 +865,7 @@
         <v>2</v>
       </c>
       <c r="I36" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J36">
         <v>2</v>
@@ -838,34 +876,34 @@
     </row>
     <row r="38" spans="3:13">
       <c r="C38" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" t="s">
+        <v>4</v>
+      </c>
+      <c r="J38" t="s">
         <v>5</v>
       </c>
-      <c r="F38" t="s">
+      <c r="K38" t="s">
         <v>6</v>
       </c>
-      <c r="G38" t="s">
+      <c r="L38" t="s">
         <v>7</v>
       </c>
-      <c r="I38" t="s">
-        <v>3</v>
-      </c>
-      <c r="J38" t="s">
-        <v>4</v>
-      </c>
-      <c r="K38" t="s">
-        <v>5</v>
-      </c>
-      <c r="L38" t="s">
-        <v>6</v>
-      </c>
       <c r="M38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="3:13">

</xml_diff>